<commit_message>
menu.php gemaakt en include jack pagina af
</commit_message>
<xml_diff>
--- a/Documents/06 Overzicht User stories.xlsx
+++ b/Documents/06 Overzicht User stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365zadkine-my.sharepoint.com/personal/0102889_zadkine_nl/Documents/Documenten/Lesmaterialen/2022-2023/Periode 03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 03\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="521" documentId="8_{32EF52FC-F33A-4C7B-AF68-432A5053B88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{023EAC7A-B6B9-4223-9B29-F9450393BDFE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A93056F-6728-4BF4-8419-2F647826679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{922DDD98-D4B6-4391-B9E3-BB09A6CA5F98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{922DDD98-D4B6-4391-B9E3-BB09A6CA5F98}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
   <si>
     <t>Teamlid</t>
   </si>
@@ -190,18 +190,6 @@
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>een positief commentaar op de website kunnen geven</t>
@@ -510,7 +498,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -526,7 +514,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -814,7 +802,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -825,7 +813,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -863,13 +851,10 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -880,18 +865,18 @@
         <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -910,9 +895,6 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -931,7 +913,7 @@
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -950,9 +932,6 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -960,22 +939,19 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -986,19 +962,16 @@
         <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -1016,9 +989,6 @@
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
@@ -1037,7 +1007,7 @@
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1056,9 +1026,6 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -1069,18 +1036,18 @@
         <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1100,7 +1067,7 @@
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1112,16 +1079,13 @@
         <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
@@ -1139,9 +1103,6 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
@@ -1152,15 +1113,15 @@
         <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -1179,9 +1140,6 @@
       </c>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
@@ -1192,19 +1150,16 @@
         <v>25</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B18" s="1">
         <v>17</v>
       </c>
@@ -1215,16 +1170,13 @@
         <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="B19" s="1">
         <v>18</v>
       </c>
@@ -1242,9 +1194,6 @@
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B20" s="1">
         <v>19</v>
       </c>
@@ -1255,18 +1204,18 @@
         <v>25</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -1285,9 +1234,6 @@
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B22" s="1">
         <v>21</v>
       </c>
@@ -1298,19 +1244,16 @@
         <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B23" s="1">
         <v>22</v>
       </c>
@@ -1321,19 +1264,16 @@
         <v>25</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="B24" s="1">
         <v>23</v>
       </c>
@@ -1344,19 +1284,16 @@
         <v>25</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B25" s="1">
         <v>24</v>
       </c>
@@ -1367,18 +1304,18 @@
         <v>25</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
@@ -1397,9 +1334,6 @@
       </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B27" s="1">
         <v>26</v>
       </c>
@@ -1417,9 +1351,6 @@
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B28" s="1">
         <v>27</v>
       </c>
@@ -1430,18 +1361,18 @@
         <v>25</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
@@ -1460,9 +1391,6 @@
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B30" s="1">
         <v>29</v>
       </c>
@@ -1473,45 +1401,39 @@
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B31" s="1">
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D31" s="1">
         <v>3</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B32" s="1">
         <v>30</v>
       </c>
@@ -1522,45 +1444,39 @@
         <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>30</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>31</v>
       </c>
@@ -1574,21 +1490,18 @@
         <v>25</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
@@ -1597,19 +1510,16 @@
         <v>25</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>32</v>
       </c>
@@ -1623,21 +1533,18 @@
         <v>25</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>32</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D37" s="1">
         <v>2</v>
@@ -1646,16 +1553,13 @@
         <v>25</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>33</v>
       </c>
@@ -1669,21 +1573,18 @@
         <v>25</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
@@ -1692,19 +1593,16 @@
         <v>25</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>34</v>
       </c>
@@ -1724,15 +1622,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>53</v>
-      </c>
+    <row r="41" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>34</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1747,10 +1642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>51</v>
-      </c>
+    <row r="42" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>35</v>
       </c>
@@ -1770,15 +1662,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>51</v>
-      </c>
+    <row r="43" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1793,10 +1682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>52</v>
-      </c>
+    <row r="44" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
         <v>36</v>
       </c>
@@ -1810,21 +1696,18 @@
         <v>25</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
+    </row>
+    <row r="45" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
         <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D45" s="1">
         <v>2</v>
@@ -1833,16 +1716,13 @@
         <v>25</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>54</v>
-      </c>
+    <row r="46" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
         <v>37</v>
       </c>
@@ -1856,21 +1736,18 @@
         <v>25</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
         <v>37</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D47" s="1">
         <v>2</v>
@@ -1879,16 +1756,13 @@
         <v>25</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
         <v>38</v>
       </c>
@@ -1902,21 +1776,18 @@
         <v>25</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>38</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D49" s="1">
         <v>2</v>
@@ -1931,10 +1802,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>52</v>
-      </c>
+    <row r="50" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>39</v>
       </c>
@@ -1945,42 +1813,36 @@
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>39</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D51" s="1">
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>54</v>
-      </c>
+    </row>
+    <row r="52" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>40</v>
       </c>
@@ -2000,15 +1862,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>54</v>
-      </c>
+    <row r="53" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>40</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D53" s="1">
         <v>2</v>
@@ -2023,10 +1882,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
-      </c>
+    <row r="54" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>41</v>
       </c>
@@ -2040,21 +1896,18 @@
         <v>25</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="1" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" s="1" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>41</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D55" s="1">
         <v>2</v>
@@ -2063,16 +1916,13 @@
         <v>25</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>42</v>
       </c>
@@ -2086,21 +1936,18 @@
         <v>25</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <v>42</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D57" s="1">
         <v>3</v>
@@ -2109,16 +1956,13 @@
         <v>25</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>43</v>
       </c>
@@ -2138,15 +1982,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>53</v>
-      </c>
+    <row r="59" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>43</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D59" s="1">
         <v>2</v>
@@ -2155,14 +1996,14 @@
         <v>25</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H59">
     <sortCondition ref="G2:G59"/>

</xml_diff>